<commit_message>
ajuste com novas planilhas
</commit_message>
<xml_diff>
--- a/download/Planilha de Inscrições Modelo EXCEL.xlsx
+++ b/download/Planilha de Inscrições Modelo EXCEL.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29030"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cabeca\Documents\planilhas de teste\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cabeca\Documents\planilhas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2D57D229-95C4-40C2-AECF-46CA8EDB7B57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BED1783C-AC0B-4EB5-BA69-1D51439F9A59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -173,6 +173,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -180,32 +183,15 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="5">
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
+          <bgColor theme="6" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -213,13 +199,6 @@
       <fill>
         <patternFill>
           <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -241,48 +220,6 @@
       <fill>
         <patternFill>
           <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -507,8 +444,8 @@
   </sheetPr>
   <dimension ref="A1:X1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1047472" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:B1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -521,20 +458,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
     </row>
     <row r="2" spans="1:24" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
     </row>
     <row r="3" spans="1:24" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
@@ -587,7 +524,7 @@
     <row r="5" spans="1:24" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="B5" s="8"/>
-      <c r="C5" s="14"/>
+      <c r="C5" s="11"/>
       <c r="D5" s="9"/>
     </row>
     <row r="6" spans="1:24" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6565,23 +6502,23 @@
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A2:D2"/>
   </mergeCells>
+  <conditionalFormatting sqref="C5:C1048576">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
+      <formula>"Feminino"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+      <formula>"Masculino"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="D5:D1048576">
-    <cfRule type="cellIs" dxfId="9" priority="5" operator="equal">
-      <formula>"Normal"</formula>
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+      <formula>"Isenta"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
       <formula>"Serviço"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
-      <formula>"Isenta"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C5:C1048576">
-    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
-      <formula>"Masculino"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
-      <formula>"Feminino"</formula>
+    <cfRule type="cellIs" dxfId="0" priority="5" operator="equal">
+      <formula>"Normal"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">

</xml_diff>